<commit_message>
add 15-5 and cp data up
</commit_message>
<xml_diff>
--- a/_back/cp/cp.xlsx
+++ b/_back/cp/cp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,10 +67,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>永远不要选自己觉得会出的号码     n+2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>忘记数据可视化图形</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -96,6 +92,34 @@
   </si>
   <si>
     <t>永远不要选择自己想要的行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>永远不要选自己觉得会出的号码     n+5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -333,7 +357,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,12 +397,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -521,13 +539,13 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -839,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V71" sqref="V71"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K73" sqref="K73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.625" defaultRowHeight="13.5"/>
@@ -4751,7 +4769,7 @@
         <v>0</v>
       </c>
       <c r="P39" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q39" s="7">
         <v>7</v>
@@ -5428,7 +5446,7 @@
         <v>3</v>
       </c>
       <c r="J46" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K46" s="7">
         <v>5</v>
@@ -5625,7 +5643,7 @@
       </c>
       <c r="J48" s="7"/>
       <c r="K48" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L48" s="7">
         <v>1</v>
@@ -5739,7 +5757,7 @@
         <v>3</v>
       </c>
       <c r="R49" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S49" s="7">
         <v>2</v>
@@ -5748,19 +5766,19 @@
         <v>0</v>
       </c>
       <c r="U49" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="V49" s="7">
         <v>2</v>
       </c>
       <c r="W49" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X49" s="42">
         <v>16</v>
       </c>
       <c r="Y49" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z49" s="7">
         <v>4</v>
@@ -5775,10 +5793,10 @@
         <v>0</v>
       </c>
       <c r="AD49" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE49" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF49" s="7">
         <v>1</v>
@@ -5789,7 +5807,7 @@
     </row>
     <row r="50" spans="1:33" s="3" customFormat="1">
       <c r="A50" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B50" s="7">
         <v>2</v>
@@ -5866,7 +5884,9 @@
       <c r="AF50" s="7">
         <v>0</v>
       </c>
-      <c r="AG50" s="7"/>
+      <c r="AG50" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:33" s="3" customFormat="1">
       <c r="A51" s="7"/>
@@ -5903,7 +5923,7 @@
         <v>4</v>
       </c>
       <c r="N51" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O51" s="7">
         <v>2</v>
@@ -5914,7 +5934,7 @@
       </c>
       <c r="R51" s="25"/>
       <c r="S51" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T51" s="7">
         <v>15</v>
@@ -5932,7 +5952,7 @@
         <v>0</v>
       </c>
       <c r="AA51" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB51" s="26">
         <v>1</v>
@@ -6011,7 +6031,7 @@
         <v>6</v>
       </c>
       <c r="AC52" s="7">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AD52" s="25"/>
       <c r="AE52" s="7"/>
@@ -6025,7 +6045,9 @@
       <c r="B53" s="26">
         <v>1</v>
       </c>
-      <c r="C53" s="7"/>
+      <c r="C53" s="7">
+        <v>0</v>
+      </c>
       <c r="D53" s="26">
         <v>5</v>
       </c>
@@ -6039,7 +6061,7 @@
         <v>5</v>
       </c>
       <c r="H53" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I53" s="7">
         <v>6</v>
@@ -6062,7 +6084,9 @@
       </c>
       <c r="R53" s="7"/>
       <c r="S53" s="7"/>
-      <c r="T53" s="7"/>
+      <c r="T53" s="7">
+        <v>0</v>
+      </c>
       <c r="U53" s="7"/>
       <c r="V53" s="7">
         <v>0</v>
@@ -6107,12 +6131,12 @@
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
       <c r="L54" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M54" s="26">
         <v>0</v>
@@ -6209,7 +6233,7 @@
       <c r="AD55" s="7"/>
       <c r="AE55" s="7"/>
       <c r="AF55" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AG55" s="7"/>
     </row>
@@ -6226,10 +6250,10 @@
         <v>6</v>
       </c>
       <c r="F56" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G56" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
@@ -6349,7 +6373,7 @@
       </c>
       <c r="N58" s="7"/>
       <c r="O58" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P58" s="7"/>
       <c r="Q58" s="7">
@@ -6364,7 +6388,7 @@
       </c>
       <c r="W58" s="7"/>
       <c r="X58" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Y58" s="28"/>
       <c r="Z58" s="7">
@@ -6398,6 +6422,9 @@
       <c r="Q59" s="7">
         <v>2</v>
       </c>
+      <c r="V59" s="7">
+        <v>0</v>
+      </c>
       <c r="Y59" s="26"/>
       <c r="Z59" s="7">
         <v>2</v>
@@ -6435,7 +6462,9 @@
     </row>
     <row r="61" spans="1:33" s="14" customFormat="1">
       <c r="A61" s="7"/>
-      <c r="B61" s="7"/>
+      <c r="B61" s="7">
+        <v>0</v>
+      </c>
       <c r="C61" s="26"/>
       <c r="D61" s="7">
         <v>0</v>
@@ -6457,7 +6486,7 @@
       <c r="O61" s="3"/>
       <c r="P61" s="26"/>
       <c r="Q61" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R61" s="7"/>
       <c r="T61" s="7"/>
@@ -6467,11 +6496,11 @@
       <c r="X61" s="3"/>
       <c r="Y61" s="7"/>
       <c r="Z61" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AA61" s="7"/>
       <c r="AB61" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC61" s="7"/>
       <c r="AE61" s="7"/>
@@ -6483,7 +6512,7 @@
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" s="7">
         <v>0</v>
@@ -6524,7 +6553,7 @@
       <c r="C63" s="5"/>
       <c r="D63" s="7"/>
       <c r="E63" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F63" s="28"/>
       <c r="G63" s="7"/>
@@ -6532,7 +6561,9 @@
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="4"/>
-      <c r="M63" s="7"/>
+      <c r="M63" s="7">
+        <v>0</v>
+      </c>
       <c r="N63" s="26"/>
       <c r="O63" s="4"/>
       <c r="P63" s="4"/>
@@ -6633,8 +6664,76 @@
       <c r="AF66" s="3"/>
       <c r="AG66" s="3"/>
     </row>
-    <row r="67" spans="1:33" s="45" customFormat="1"/>
-    <row r="68" spans="1:33" s="43" customFormat="1"/>
+    <row r="67" spans="1:33" s="45" customFormat="1">
+      <c r="A67" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="L67" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="O67" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q67" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="R67" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="V67" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="X67" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y67" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z67" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF67" s="45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:33" s="43" customFormat="1">
+      <c r="C68" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="D68" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="J68" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="K68" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="M68" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="U68" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="W68" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB68" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE68" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG68" s="43" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="69" spans="1:33" s="47" customFormat="1"/>
     <row r="70" spans="1:33">
       <c r="C70" s="5"/>
@@ -7361,8 +7460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD976"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V132" sqref="V132"/>
+    <sheetView topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U132" sqref="U132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5"/>
@@ -14715,7 +14814,7 @@
       <c r="S98" s="19">
         <v>4</v>
       </c>
-      <c r="T98" s="61">
+      <c r="T98" s="19">
         <v>27</v>
       </c>
       <c r="U98" s="19">
@@ -14870,7 +14969,7 @@
         <v>4</v>
       </c>
       <c r="T100" s="20">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="U100" s="19">
         <v>1</v>
@@ -15641,7 +15740,7 @@
         <v>3</v>
       </c>
       <c r="U110" s="23">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="V110" s="22">
         <v>5</v>
@@ -16018,7 +16117,7 @@
         <v>0</v>
       </c>
       <c r="S115" s="23">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T115" s="22">
         <v>2</v>
@@ -16093,7 +16192,7 @@
         <v>2</v>
       </c>
       <c r="S116" s="23">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T116" s="22">
         <v>2</v>
@@ -16165,13 +16264,13 @@
         <v>6</v>
       </c>
       <c r="R117" s="23">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="S117" s="22">
         <v>2</v>
       </c>
       <c r="T117" s="23">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="U117" s="22">
         <v>3</v>
@@ -16249,7 +16348,7 @@
       <c r="U118" s="22">
         <v>0</v>
       </c>
-      <c r="V118" s="60">
+      <c r="V118" s="22">
         <v>7</v>
       </c>
       <c r="W118" s="23"/>
@@ -16316,17 +16415,17 @@
       <c r="R119" s="22">
         <v>2</v>
       </c>
-      <c r="S119" s="23">
+      <c r="S119" s="22">
         <v>7</v>
       </c>
-      <c r="T119" s="23">
+      <c r="T119" s="22">
         <v>7</v>
       </c>
       <c r="U119" s="22">
         <v>2</v>
       </c>
       <c r="V119" s="23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="W119" s="23"/>
       <c r="X119" s="21">
@@ -16338,8 +16437,12 @@
       <c r="Z119" s="21">
         <v>2</v>
       </c>
-      <c r="AA119" s="41"/>
-      <c r="AB119" s="41"/>
+      <c r="AA119" s="21">
+        <v>7</v>
+      </c>
+      <c r="AB119" s="21">
+        <v>7</v>
+      </c>
       <c r="AC119" s="41"/>
     </row>
     <row r="120" spans="1:30" s="21" customFormat="1">
@@ -16395,7 +16498,7 @@
       <c r="U120" s="22">
         <v>3</v>
       </c>
-      <c r="V120" s="60">
+      <c r="V120" s="22">
         <v>5</v>
       </c>
       <c r="W120" s="23"/>
@@ -16460,7 +16563,7 @@
         <v>3</v>
       </c>
       <c r="R121" s="23">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S121" s="22">
         <v>1</v>
@@ -16531,21 +16634,21 @@
       </c>
       <c r="P122" s="22"/>
       <c r="Q122" s="23">
-        <v>4</v>
-      </c>
-      <c r="R122" s="60">
-        <v>3</v>
-      </c>
-      <c r="S122" s="23">
+        <v>5</v>
+      </c>
+      <c r="R122" s="22">
+        <v>3</v>
+      </c>
+      <c r="S122" s="22">
         <v>4</v>
       </c>
       <c r="T122" s="22">
         <v>1</v>
       </c>
       <c r="U122" s="23">
-        <v>4</v>
-      </c>
-      <c r="V122" s="60">
+        <v>5</v>
+      </c>
+      <c r="V122" s="22">
         <v>3</v>
       </c>
       <c r="W122" s="23"/>
@@ -16558,7 +16661,9 @@
       <c r="Z122" s="21">
         <v>3</v>
       </c>
-      <c r="AA122" s="41"/>
+      <c r="AA122" s="21">
+        <v>4</v>
+      </c>
       <c r="AB122" s="41"/>
       <c r="AC122" s="41"/>
     </row>
@@ -16599,20 +16704,21 @@
       <c r="N123" s="21">
         <v>10</v>
       </c>
+      <c r="P123" s="22"/>
       <c r="Q123" s="23">
-        <v>3</v>
-      </c>
-      <c r="R123" s="23">
+        <v>4</v>
+      </c>
+      <c r="R123" s="22">
         <v>3</v>
       </c>
       <c r="S123" s="22">
         <v>1</v>
       </c>
       <c r="T123" s="23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U123" s="23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V123" s="22">
         <v>0</v>
@@ -16624,7 +16730,9 @@
       <c r="Y123" s="21">
         <v>1</v>
       </c>
-      <c r="Z123" s="41"/>
+      <c r="Z123" s="21">
+        <v>3</v>
+      </c>
       <c r="AA123" s="41"/>
       <c r="AB123" s="41"/>
       <c r="AC123" s="41"/>
@@ -16667,29 +16775,31 @@
         <v>17</v>
       </c>
       <c r="P124" s="22"/>
-      <c r="Q124" s="23">
+      <c r="Q124" s="22">
         <v>2</v>
       </c>
       <c r="R124" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S124" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T124" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U124" s="22">
         <v>0</v>
       </c>
       <c r="V124" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W124" s="41"/>
       <c r="X124" s="21">
         <v>0</v>
       </c>
-      <c r="Y124" s="41"/>
+      <c r="Y124" s="21">
+        <v>2</v>
+      </c>
       <c r="Z124" s="41"/>
       <c r="AA124" s="41"/>
       <c r="AB124" s="41"/>
@@ -16732,23 +16842,24 @@
       <c r="N125" s="21">
         <v>16</v>
       </c>
-      <c r="Q125" s="60">
+      <c r="P125" s="22"/>
+      <c r="Q125" s="22">
         <v>0</v>
       </c>
       <c r="R125" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S125" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T125" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U125" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V125" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W125" s="23"/>
       <c r="X125" s="21">
@@ -16799,25 +16910,27 @@
       </c>
       <c r="P126" s="22"/>
       <c r="Q126" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R126" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S126" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T126" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U126" s="23">
-        <v>0</v>
-      </c>
-      <c r="V126" s="23">
+        <v>1</v>
+      </c>
+      <c r="V126" s="22">
         <v>0</v>
       </c>
       <c r="W126" s="41"/>
-      <c r="X126" s="41"/>
+      <c r="X126" s="21">
+        <v>0</v>
+      </c>
       <c r="Y126" s="41"/>
       <c r="Z126" s="41"/>
       <c r="AA126" s="41"/>
@@ -16826,13 +16939,61 @@
       <c r="AD126" s="41"/>
     </row>
     <row r="127" spans="1:30" s="21" customFormat="1">
+      <c r="A127" s="21">
+        <v>3</v>
+      </c>
+      <c r="B127" s="21">
+        <v>2</v>
+      </c>
+      <c r="C127" s="21">
+        <v>4</v>
+      </c>
+      <c r="D127" s="21">
+        <v>7</v>
+      </c>
+      <c r="E127" s="21">
+        <v>7</v>
+      </c>
+      <c r="F127" s="21">
+        <v>0</v>
+      </c>
+      <c r="I127" s="21">
+        <v>0</v>
+      </c>
+      <c r="J127" s="21">
+        <v>2</v>
+      </c>
+      <c r="K127" s="21">
+        <v>3</v>
+      </c>
+      <c r="L127" s="21">
+        <v>4</v>
+      </c>
+      <c r="M127" s="21">
+        <v>7</v>
+      </c>
+      <c r="N127" s="21">
+        <v>7</v>
+      </c>
       <c r="P127" s="22"/>
-      <c r="Q127" s="23"/>
-      <c r="R127" s="23"/>
-      <c r="S127" s="23"/>
-      <c r="T127" s="23"/>
-      <c r="U127" s="23"/>
-      <c r="V127" s="23"/>
+      <c r="Q127" s="23">
+        <v>0</v>
+      </c>
+      <c r="R127" s="23">
+        <v>0</v>
+      </c>
+      <c r="S127" s="23">
+        <v>0</v>
+      </c>
+      <c r="T127" s="23">
+        <v>0</v>
+      </c>
+      <c r="U127" s="23">
+        <v>0</v>
+      </c>
+      <c r="V127" s="23">
+        <v>0</v>
+      </c>
       <c r="W127" s="41"/>
       <c r="X127" s="41"/>
       <c r="Y127" s="41"/>
@@ -17124,7 +17285,7 @@
       <c r="AC144" s="41"/>
       <c r="AD144" s="41"/>
     </row>
-    <row r="145" spans="9:30" s="21" customFormat="1">
+    <row r="145" spans="16:30" s="21" customFormat="1">
       <c r="P145" s="22"/>
       <c r="Q145" s="23"/>
       <c r="R145" s="23"/>
@@ -17141,7 +17302,7 @@
       <c r="AC145" s="41"/>
       <c r="AD145" s="41"/>
     </row>
-    <row r="146" spans="9:30" s="21" customFormat="1">
+    <row r="146" spans="16:30" s="21" customFormat="1">
       <c r="P146" s="22"/>
       <c r="Q146" s="23"/>
       <c r="R146" s="23"/>
@@ -17158,7 +17319,7 @@
       <c r="AC146" s="41"/>
       <c r="AD146" s="41"/>
     </row>
-    <row r="147" spans="9:30" s="21" customFormat="1">
+    <row r="147" spans="16:30" s="21" customFormat="1">
       <c r="P147" s="22"/>
       <c r="Q147" s="23"/>
       <c r="R147" s="23"/>
@@ -17175,7 +17336,7 @@
       <c r="AC147" s="23"/>
       <c r="AD147" s="41"/>
     </row>
-    <row r="148" spans="9:30" s="21" customFormat="1">
+    <row r="148" spans="16:30" s="21" customFormat="1">
       <c r="P148" s="22"/>
       <c r="Q148" s="23"/>
       <c r="R148" s="23"/>
@@ -17192,25 +17353,7 @@
       <c r="AC148" s="41"/>
       <c r="AD148" s="41"/>
     </row>
-    <row r="149" spans="9:30" s="21" customFormat="1">
-      <c r="I149" s="21">
-        <v>0</v>
-      </c>
-      <c r="J149" s="21">
-        <v>3</v>
-      </c>
-      <c r="K149" s="21">
-        <v>3</v>
-      </c>
-      <c r="L149" s="21">
-        <v>6</v>
-      </c>
-      <c r="M149" s="21">
-        <v>8</v>
-      </c>
-      <c r="N149" s="21">
-        <v>15</v>
-      </c>
+    <row r="149" spans="16:30" s="21" customFormat="1">
       <c r="P149" s="22"/>
       <c r="Q149" s="23"/>
       <c r="R149" s="23"/>
@@ -17227,7 +17370,7 @@
       <c r="AC149" s="41"/>
       <c r="AD149" s="41"/>
     </row>
-    <row r="150" spans="9:30" s="21" customFormat="1">
+    <row r="150" spans="16:30" s="21" customFormat="1">
       <c r="P150" s="22"/>
       <c r="Q150" s="23"/>
       <c r="R150" s="23"/>
@@ -17244,7 +17387,7 @@
       <c r="AC150" s="23"/>
       <c r="AD150" s="41"/>
     </row>
-    <row r="151" spans="9:30" s="21" customFormat="1">
+    <row r="151" spans="16:30" s="21" customFormat="1">
       <c r="P151" s="22"/>
       <c r="Q151" s="23"/>
       <c r="R151" s="23"/>
@@ -17261,25 +17404,7 @@
       <c r="AC151" s="41"/>
       <c r="AD151" s="41"/>
     </row>
-    <row r="152" spans="9:30" s="21" customFormat="1">
-      <c r="I152" s="21">
-        <v>0</v>
-      </c>
-      <c r="J152" s="21">
-        <v>0</v>
-      </c>
-      <c r="K152" s="21">
-        <v>0</v>
-      </c>
-      <c r="L152" s="21">
-        <v>1</v>
-      </c>
-      <c r="M152" s="21">
-        <v>3</v>
-      </c>
-      <c r="N152" s="21">
-        <v>15</v>
-      </c>
+    <row r="152" spans="16:30" s="21" customFormat="1">
       <c r="P152" s="22"/>
       <c r="Q152" s="23"/>
       <c r="R152" s="23"/>
@@ -17296,7 +17421,7 @@
       <c r="AC152" s="41"/>
       <c r="AD152" s="41"/>
     </row>
-    <row r="153" spans="9:30" s="21" customFormat="1">
+    <row r="153" spans="16:30" s="21" customFormat="1">
       <c r="Q153" s="23"/>
       <c r="R153" s="23"/>
       <c r="S153" s="23"/>
@@ -17312,25 +17437,7 @@
       <c r="AC153" s="41"/>
       <c r="AD153" s="41"/>
     </row>
-    <row r="154" spans="9:30" s="21" customFormat="1">
-      <c r="I154" s="21">
-        <v>0</v>
-      </c>
-      <c r="J154" s="21">
-        <v>1</v>
-      </c>
-      <c r="K154" s="21">
-        <v>3</v>
-      </c>
-      <c r="L154" s="21">
-        <v>3</v>
-      </c>
-      <c r="M154" s="21">
-        <v>6</v>
-      </c>
-      <c r="N154" s="21">
-        <v>25</v>
-      </c>
+    <row r="154" spans="16:30" s="21" customFormat="1">
       <c r="P154" s="22"/>
       <c r="Q154" s="23"/>
       <c r="R154" s="23"/>
@@ -17347,7 +17454,7 @@
       <c r="AC154" s="41"/>
       <c r="AD154" s="41"/>
     </row>
-    <row r="155" spans="9:30" s="21" customFormat="1">
+    <row r="155" spans="16:30" s="21" customFormat="1">
       <c r="Q155" s="23"/>
       <c r="R155" s="23"/>
       <c r="S155" s="23"/>
@@ -17363,22 +17470,7 @@
       <c r="AC155" s="23"/>
       <c r="AD155" s="41"/>
     </row>
-    <row r="156" spans="9:30" s="21" customFormat="1">
-      <c r="I156" s="21">
-        <v>1</v>
-      </c>
-      <c r="J156" s="21">
-        <v>3</v>
-      </c>
-      <c r="K156" s="21">
-        <v>3</v>
-      </c>
-      <c r="L156" s="21">
-        <v>6</v>
-      </c>
-      <c r="M156" s="21">
-        <v>25</v>
-      </c>
+    <row r="156" spans="16:30" s="21" customFormat="1">
       <c r="P156" s="22"/>
       <c r="Q156" s="23"/>
       <c r="R156" s="23"/>
@@ -17395,7 +17487,7 @@
       <c r="AC156" s="41"/>
       <c r="AD156" s="41"/>
     </row>
-    <row r="157" spans="9:30" s="21" customFormat="1">
+    <row r="157" spans="16:30" s="21" customFormat="1">
       <c r="Q157" s="23"/>
       <c r="R157" s="23"/>
       <c r="S157" s="23"/>
@@ -17411,25 +17503,7 @@
       <c r="AC157" s="23"/>
       <c r="AD157" s="41"/>
     </row>
-    <row r="158" spans="9:30" s="21" customFormat="1">
-      <c r="I158" s="21">
-        <v>1</v>
-      </c>
-      <c r="J158" s="21">
-        <v>3</v>
-      </c>
-      <c r="K158" s="21">
-        <v>3</v>
-      </c>
-      <c r="L158" s="21">
-        <v>5</v>
-      </c>
-      <c r="M158" s="21">
-        <v>6</v>
-      </c>
-      <c r="N158" s="21">
-        <v>25</v>
-      </c>
+    <row r="158" spans="16:30" s="21" customFormat="1">
       <c r="Q158" s="23"/>
       <c r="R158" s="23"/>
       <c r="S158" s="23"/>
@@ -17445,7 +17519,7 @@
       <c r="AC158" s="23"/>
       <c r="AD158" s="41"/>
     </row>
-    <row r="159" spans="9:30" s="21" customFormat="1">
+    <row r="159" spans="16:30" s="21" customFormat="1">
       <c r="P159" s="22"/>
       <c r="Q159" s="23"/>
       <c r="R159" s="23"/>
@@ -17462,25 +17536,7 @@
       <c r="AC159" s="41"/>
       <c r="AD159" s="41"/>
     </row>
-    <row r="160" spans="9:30" s="21" customFormat="1">
-      <c r="I160" s="21">
-        <v>1</v>
-      </c>
-      <c r="J160" s="21">
-        <v>2</v>
-      </c>
-      <c r="K160" s="21">
-        <v>6</v>
-      </c>
-      <c r="L160" s="21">
-        <v>6</v>
-      </c>
-      <c r="M160" s="21">
-        <v>8</v>
-      </c>
-      <c r="N160" s="21">
-        <v>8</v>
-      </c>
+    <row r="160" spans="16:30" s="21" customFormat="1">
       <c r="Q160" s="23"/>
       <c r="R160" s="23"/>
       <c r="S160" s="23"/>
@@ -30034,10 +30090,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO183"/>
+  <dimension ref="A1:AO184"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K132" sqref="K132"/>
+    <sheetView topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L132" sqref="L132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.625" defaultRowHeight="13.5"/>
@@ -32582,10 +32638,10 @@
       </c>
     </row>
     <row r="126" spans="1:41">
-      <c r="A126" s="10"/>
-      <c r="B126" s="9">
-        <v>1</v>
-      </c>
+      <c r="A126" s="9">
+        <v>1</v>
+      </c>
+      <c r="B126" s="10"/>
       <c r="C126" s="10"/>
       <c r="D126" s="11">
         <v>2</v>
@@ -32612,16 +32668,39 @@
       </c>
     </row>
     <row r="127" spans="1:41">
-      <c r="A127" s="10"/>
+      <c r="A127" s="9">
+        <v>1</v>
+      </c>
       <c r="B127" s="10"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
-      <c r="E127" s="10"/>
+      <c r="C127" s="9">
+        <v>1</v>
+      </c>
+      <c r="D127" s="9">
+        <v>1</v>
+      </c>
+      <c r="E127" s="9">
+        <v>1</v>
+      </c>
       <c r="F127" s="10"/>
       <c r="G127" s="10"/>
+      <c r="H127" s="11">
+        <v>2</v>
+      </c>
       <c r="I127" s="10"/>
       <c r="J127" s="10"/>
       <c r="K127" s="10"/>
+      <c r="L127" s="10"/>
+      <c r="Q127" s="10"/>
+      <c r="R127" s="18"/>
+      <c r="S127" s="18"/>
+      <c r="T127" s="18"/>
+      <c r="U127" s="18"/>
+      <c r="V127" s="18"/>
+      <c r="W127" s="18"/>
+      <c r="X127" s="18"/>
+      <c r="Y127" s="18"/>
+      <c r="Z127" s="18"/>
+      <c r="AA127" s="10"/>
     </row>
     <row r="128" spans="1:41">
       <c r="A128" s="10"/>
@@ -32631,9 +32710,10 @@
       <c r="E128" s="10"/>
       <c r="F128" s="10"/>
       <c r="G128" s="10"/>
+      <c r="H128" s="10"/>
       <c r="J128" s="10"/>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:8">
       <c r="A129" s="10"/>
       <c r="B129" s="10"/>
       <c r="C129" s="10"/>
@@ -32641,8 +32721,9 @@
       <c r="E129" s="10"/>
       <c r="F129" s="10"/>
       <c r="G129" s="10"/>
-    </row>
-    <row r="130" spans="1:7">
+      <c r="H129" s="10"/>
+    </row>
+    <row r="130" spans="1:8">
       <c r="A130" s="10"/>
       <c r="B130" s="10"/>
       <c r="C130" s="10"/>
@@ -32650,7 +32731,7 @@
       <c r="E130" s="10"/>
       <c r="F130" s="10"/>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:8">
       <c r="A131" s="10"/>
       <c r="B131" s="10"/>
       <c r="C131" s="10"/>
@@ -32658,7 +32739,7 @@
       <c r="E131" s="10"/>
       <c r="F131" s="10"/>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:8">
       <c r="A132" s="10"/>
       <c r="B132" s="10"/>
       <c r="C132" s="10"/>
@@ -32666,7 +32747,7 @@
       <c r="E132" s="10"/>
       <c r="F132" s="10"/>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:8">
       <c r="A133" s="10"/>
       <c r="B133" s="10"/>
       <c r="C133" s="10"/>
@@ -32674,7 +32755,7 @@
       <c r="E133" s="10"/>
       <c r="F133" s="10"/>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:8">
       <c r="A134" s="10"/>
       <c r="B134" s="10"/>
       <c r="C134" s="10"/>
@@ -32682,7 +32763,7 @@
       <c r="E134" s="10"/>
       <c r="F134" s="10"/>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:8">
       <c r="A135" s="10"/>
       <c r="B135" s="10"/>
       <c r="C135" s="10"/>
@@ -32690,7 +32771,7 @@
       <c r="E135" s="10"/>
       <c r="F135" s="10"/>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:8">
       <c r="A136" s="10"/>
       <c r="B136" s="10"/>
       <c r="C136" s="10"/>
@@ -32698,7 +32779,7 @@
       <c r="E136" s="10"/>
       <c r="F136" s="10"/>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:8">
       <c r="A137" s="10"/>
       <c r="B137" s="10"/>
       <c r="C137" s="10"/>
@@ -32706,7 +32787,7 @@
       <c r="E137" s="10"/>
       <c r="F137" s="10"/>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:8">
       <c r="A138" s="10"/>
       <c r="B138" s="10"/>
       <c r="C138" s="10"/>
@@ -32714,7 +32795,7 @@
       <c r="E138" s="10"/>
       <c r="F138" s="10"/>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:8">
       <c r="A139" s="10"/>
       <c r="B139" s="10"/>
       <c r="C139" s="10"/>
@@ -32722,7 +32803,7 @@
       <c r="E139" s="10"/>
       <c r="F139" s="10"/>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:8">
       <c r="A140" s="10"/>
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
@@ -32730,7 +32811,7 @@
       <c r="E140" s="10"/>
       <c r="F140" s="10"/>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:8">
       <c r="A141" s="10"/>
       <c r="B141" s="10"/>
       <c r="C141" s="10"/>
@@ -32738,7 +32819,7 @@
       <c r="E141" s="10"/>
       <c r="F141" s="10"/>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:8">
       <c r="A142" s="10"/>
       <c r="B142" s="10"/>
       <c r="C142" s="10"/>
@@ -32746,7 +32827,7 @@
       <c r="E142" s="10"/>
       <c r="F142" s="10"/>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:8">
       <c r="A143" s="10"/>
       <c r="B143" s="10"/>
       <c r="C143" s="10"/>
@@ -32754,7 +32835,7 @@
       <c r="E143" s="10"/>
       <c r="F143" s="10"/>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:8">
       <c r="A144" s="10"/>
       <c r="B144" s="10"/>
       <c r="C144" s="10"/>
@@ -32783,6 +32864,7 @@
       <c r="B147" s="10"/>
       <c r="C147" s="10"/>
       <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
       <c r="F147" s="10"/>
     </row>
     <row r="148" spans="1:6">
@@ -32790,6 +32872,7 @@
       <c r="B148" s="10"/>
       <c r="C148" s="10"/>
       <c r="D148" s="10"/>
+      <c r="E148" s="10"/>
       <c r="F148" s="10"/>
     </row>
     <row r="149" spans="1:6">
@@ -32864,6 +32947,7 @@
     </row>
     <row r="159" spans="1:6">
       <c r="A159" s="10"/>
+      <c r="B159" s="10"/>
       <c r="C159" s="10"/>
       <c r="D159" s="10"/>
       <c r="F159" s="10"/>
@@ -32959,30 +33043,38 @@
     <row r="175" spans="1:6">
       <c r="A175" s="10"/>
       <c r="C175" s="10"/>
+      <c r="D175" s="10"/>
     </row>
     <row r="176" spans="1:6">
+      <c r="A176" s="10"/>
       <c r="C176" s="10"/>
-    </row>
-    <row r="177" spans="3:3">
+      <c r="D176" s="10"/>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" s="10"/>
       <c r="C177" s="10"/>
     </row>
-    <row r="178" spans="3:3">
+    <row r="178" spans="1:3">
+      <c r="A178" s="10"/>
       <c r="C178" s="10"/>
     </row>
-    <row r="179" spans="3:3">
+    <row r="179" spans="1:3">
       <c r="C179" s="10"/>
     </row>
-    <row r="180" spans="3:3">
+    <row r="180" spans="1:3">
       <c r="C180" s="10"/>
     </row>
-    <row r="181" spans="3:3">
+    <row r="181" spans="1:3">
       <c r="C181" s="10"/>
     </row>
-    <row r="182" spans="3:3">
+    <row r="182" spans="1:3">
       <c r="C182" s="10"/>
     </row>
-    <row r="183" spans="3:3">
+    <row r="183" spans="1:3">
       <c r="C183" s="10"/>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="C184" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -32993,10 +33085,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S183"/>
+  <dimension ref="A1:S201"/>
   <sheetViews>
-    <sheetView topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="E130" sqref="E130"/>
+    <sheetView topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="P134" sqref="P134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -35210,88 +35302,169 @@
         <v>40</v>
       </c>
     </row>
-    <row r="129" spans="1:12">
-      <c r="F129" s="18"/>
-      <c r="G129" s="18"/>
-      <c r="H129" s="18"/>
-      <c r="I129" s="18"/>
-      <c r="J129" s="18"/>
-      <c r="K129" s="18"/>
-      <c r="L129" s="18"/>
-    </row>
-    <row r="130" spans="1:12">
-      <c r="F130" s="18"/>
-      <c r="G130" s="18"/>
-      <c r="H130" s="18"/>
-      <c r="I130" s="18"/>
-      <c r="J130" s="18"/>
-      <c r="K130" s="18"/>
-      <c r="L130" s="18"/>
-    </row>
-    <row r="138" spans="1:12">
-      <c r="A138" s="37"/>
-      <c r="B138" s="37"/>
-      <c r="C138" s="37"/>
-    </row>
-    <row r="139" spans="1:12">
-      <c r="A139" s="37"/>
-      <c r="B139" s="37"/>
-      <c r="C139" s="37"/>
-    </row>
-    <row r="146" spans="6:19">
-      <c r="N146" s="18"/>
-      <c r="O146" s="18"/>
-      <c r="P146" s="18"/>
-      <c r="Q146" s="18"/>
-      <c r="R146" s="18"/>
-      <c r="S146" s="18"/>
-    </row>
-    <row r="152" spans="6:19">
-      <c r="F152" s="18"/>
-      <c r="G152" s="18"/>
-      <c r="H152" s="18"/>
-      <c r="I152" s="18"/>
-      <c r="J152" s="18"/>
-      <c r="K152" s="18"/>
-      <c r="L152" s="18"/>
-    </row>
-    <row r="153" spans="6:19">
-      <c r="F153" s="18"/>
-      <c r="G153" s="18"/>
-      <c r="H153" s="18"/>
-      <c r="I153" s="18"/>
-      <c r="J153" s="18"/>
-      <c r="K153" s="18"/>
-      <c r="L153" s="18"/>
-    </row>
-    <row r="161" spans="1:19">
-      <c r="A161" s="37"/>
-      <c r="B161" s="37"/>
-      <c r="C161" s="37"/>
-    </row>
-    <row r="168" spans="1:19">
-      <c r="N168" s="18"/>
-      <c r="O168" s="18"/>
-      <c r="P168" s="18"/>
-      <c r="Q168" s="18"/>
-      <c r="R168" s="18"/>
-      <c r="S168" s="18"/>
-    </row>
-    <row r="181" spans="14:19">
-      <c r="N181" s="18"/>
-      <c r="O181" s="18"/>
-      <c r="P181" s="18"/>
-      <c r="Q181" s="18"/>
-      <c r="R181" s="18"/>
-      <c r="S181" s="18"/>
-    </row>
-    <row r="183" spans="14:19">
-      <c r="N183" s="18"/>
-      <c r="O183" s="18"/>
-      <c r="P183" s="18"/>
-      <c r="Q183" s="18"/>
-      <c r="R183" s="18"/>
-      <c r="S183" s="18"/>
+    <row r="127" spans="1:19">
+      <c r="A127" s="1">
+        <v>1</v>
+      </c>
+      <c r="B127" s="1">
+        <v>2</v>
+      </c>
+      <c r="C127" s="1">
+        <v>3</v>
+      </c>
+      <c r="F127" s="1">
+        <v>1</v>
+      </c>
+      <c r="G127" s="1">
+        <v>1</v>
+      </c>
+      <c r="H127" s="1">
+        <v>2</v>
+      </c>
+      <c r="I127" s="1">
+        <v>1</v>
+      </c>
+      <c r="J127" s="1">
+        <v>0</v>
+      </c>
+      <c r="K127" s="1">
+        <v>1</v>
+      </c>
+      <c r="N127" s="18">
+        <v>0</v>
+      </c>
+      <c r="O127" s="18">
+        <v>1</v>
+      </c>
+      <c r="P127" s="18">
+        <v>4</v>
+      </c>
+      <c r="Q127" s="18">
+        <v>5</v>
+      </c>
+      <c r="R127" s="18">
+        <v>7</v>
+      </c>
+      <c r="S127" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19">
+      <c r="A133" s="37"/>
+      <c r="B133" s="37"/>
+      <c r="C133" s="37"/>
+    </row>
+    <row r="134" spans="1:19">
+      <c r="A134" s="37"/>
+      <c r="B134" s="37"/>
+      <c r="C134" s="37"/>
+    </row>
+    <row r="141" spans="1:19">
+      <c r="N141" s="18"/>
+      <c r="O141" s="18"/>
+      <c r="P141" s="18"/>
+      <c r="Q141" s="18"/>
+      <c r="R141" s="18"/>
+      <c r="S141" s="18"/>
+    </row>
+    <row r="147" spans="1:12">
+      <c r="F147" s="18"/>
+      <c r="G147" s="18"/>
+      <c r="H147" s="18"/>
+      <c r="I147" s="18"/>
+      <c r="J147" s="18"/>
+      <c r="K147" s="18"/>
+      <c r="L147" s="18"/>
+    </row>
+    <row r="148" spans="1:12">
+      <c r="F148" s="18"/>
+      <c r="G148" s="18"/>
+      <c r="H148" s="18"/>
+      <c r="I148" s="18"/>
+      <c r="J148" s="18"/>
+      <c r="K148" s="18"/>
+      <c r="L148" s="18"/>
+    </row>
+    <row r="149" spans="1:12">
+      <c r="B149" s="1">
+        <v>1</v>
+      </c>
+      <c r="C149" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12">
+      <c r="B150" s="1">
+        <v>2</v>
+      </c>
+      <c r="C150" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12">
+      <c r="A156" s="37"/>
+      <c r="B156" s="37"/>
+      <c r="C156" s="37"/>
+    </row>
+    <row r="157" spans="1:12">
+      <c r="A157" s="37"/>
+      <c r="B157" s="37"/>
+      <c r="C157" s="37"/>
+    </row>
+    <row r="164" spans="6:19">
+      <c r="N164" s="18"/>
+      <c r="O164" s="18"/>
+      <c r="P164" s="18"/>
+      <c r="Q164" s="18"/>
+      <c r="R164" s="18"/>
+      <c r="S164" s="18"/>
+    </row>
+    <row r="170" spans="6:19">
+      <c r="F170" s="18"/>
+      <c r="G170" s="18"/>
+      <c r="H170" s="18"/>
+      <c r="I170" s="18"/>
+      <c r="J170" s="18"/>
+      <c r="K170" s="18"/>
+      <c r="L170" s="18"/>
+    </row>
+    <row r="171" spans="6:19">
+      <c r="F171" s="18"/>
+      <c r="G171" s="18"/>
+      <c r="H171" s="18"/>
+      <c r="I171" s="18"/>
+      <c r="J171" s="18"/>
+      <c r="K171" s="18"/>
+      <c r="L171" s="18"/>
+    </row>
+    <row r="179" spans="1:19">
+      <c r="A179" s="37"/>
+      <c r="B179" s="37"/>
+      <c r="C179" s="37"/>
+    </row>
+    <row r="186" spans="1:19">
+      <c r="N186" s="18"/>
+      <c r="O186" s="18"/>
+      <c r="P186" s="18"/>
+      <c r="Q186" s="18"/>
+      <c r="R186" s="18"/>
+      <c r="S186" s="18"/>
+    </row>
+    <row r="199" spans="14:19">
+      <c r="N199" s="18"/>
+      <c r="O199" s="18"/>
+      <c r="P199" s="18"/>
+      <c r="Q199" s="18"/>
+      <c r="R199" s="18"/>
+      <c r="S199" s="18"/>
+    </row>
+    <row r="201" spans="14:19">
+      <c r="N201" s="18"/>
+      <c r="O201" s="18"/>
+      <c r="P201" s="18"/>
+      <c r="Q201" s="18"/>
+      <c r="R201" s="18"/>
+      <c r="S201" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -35302,10 +35475,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A100:AR128"/>
+  <dimension ref="A100:AR129"/>
   <sheetViews>
     <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="H134" sqref="H134"/>
+      <selection activeCell="D127" sqref="D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -36900,13 +37073,45 @@
       </c>
     </row>
     <row r="127" spans="1:44">
-      <c r="A127" s="10"/>
+      <c r="A127" s="9">
+        <v>1</v>
+      </c>
+      <c r="C127" s="11">
+        <v>2</v>
+      </c>
+      <c r="D127" s="11">
+        <v>3</v>
+      </c>
       <c r="E127" s="10"/>
       <c r="F127" s="10"/>
       <c r="J127" s="10"/>
+      <c r="P127" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q127" s="16">
+        <v>2</v>
+      </c>
+      <c r="R127" s="16">
+        <v>2</v>
+      </c>
+      <c r="S127" s="16">
+        <v>3</v>
+      </c>
+      <c r="T127" s="16">
+        <v>3</v>
+      </c>
+      <c r="U127" s="16">
+        <v>3</v>
+      </c>
+      <c r="W127" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="128" spans="1:44">
       <c r="A128" s="10"/>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -36919,15 +37124,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="5" width="6.625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="6.625" style="59" customWidth="1"/>
-    <col min="7" max="16" width="6.625" style="18" customWidth="1"/>
+    <col min="1" max="4" width="6.625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="6.625" style="60" customWidth="1"/>
+    <col min="6" max="6" width="6.625" style="61" customWidth="1"/>
+    <col min="7" max="7" width="6.625" style="18" customWidth="1"/>
+    <col min="8" max="10" width="6.625" style="60" customWidth="1"/>
+    <col min="11" max="11" width="6.625" style="18" customWidth="1"/>
+    <col min="12" max="13" width="6.625" style="60" customWidth="1"/>
+    <col min="14" max="14" width="6.625" style="18" customWidth="1"/>
+    <col min="15" max="15" width="6.625" style="60" customWidth="1"/>
+    <col min="16" max="16" width="6.625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -36943,37 +37155,37 @@
       <c r="D1" s="18">
         <v>47</v>
       </c>
-      <c r="E1" s="18">
+      <c r="E1" s="60">
         <v>41</v>
       </c>
-      <c r="F1" s="59">
+      <c r="F1" s="61">
         <v>17</v>
       </c>
       <c r="G1" s="18">
         <v>23</v>
       </c>
-      <c r="H1" s="18">
+      <c r="H1" s="60">
         <v>10</v>
       </c>
-      <c r="I1" s="18">
-        <v>3</v>
-      </c>
-      <c r="J1" s="18">
+      <c r="I1" s="60">
+        <v>3</v>
+      </c>
+      <c r="J1" s="60">
         <v>40</v>
       </c>
       <c r="K1" s="18">
         <v>38</v>
       </c>
-      <c r="L1" s="18">
+      <c r="L1" s="60">
         <v>16</v>
       </c>
-      <c r="M1" s="18">
+      <c r="M1" s="60">
         <v>21</v>
       </c>
       <c r="N1" s="18">
         <v>52</v>
       </c>
-      <c r="O1" s="18">
+      <c r="O1" s="60">
         <v>15</v>
       </c>
       <c r="P1" s="18">
@@ -36991,39 +37203,39 @@
         <v>0</v>
       </c>
       <c r="D2" s="18">
-        <v>78</v>
-      </c>
-      <c r="E2" s="18">
-        <v>1</v>
-      </c>
-      <c r="F2" s="59">
+        <v>79</v>
+      </c>
+      <c r="E2" s="60">
+        <v>1</v>
+      </c>
+      <c r="F2" s="61">
         <v>10</v>
       </c>
       <c r="G2" s="18">
         <v>43</v>
       </c>
-      <c r="H2" s="18">
+      <c r="H2" s="60">
         <v>64</v>
       </c>
-      <c r="I2" s="18">
+      <c r="I2" s="60">
         <v>6</v>
       </c>
-      <c r="J2" s="18">
+      <c r="J2" s="60">
         <v>50</v>
       </c>
       <c r="K2" s="18">
         <v>4</v>
       </c>
-      <c r="L2" s="18">
-        <v>1</v>
-      </c>
-      <c r="M2" s="18">
+      <c r="L2" s="60">
+        <v>1</v>
+      </c>
+      <c r="M2" s="60">
         <v>7</v>
       </c>
       <c r="N2" s="18">
         <v>11</v>
       </c>
-      <c r="O2" s="18">
+      <c r="O2" s="60">
         <v>6</v>
       </c>
       <c r="P2" s="18">
@@ -37040,37 +37252,37 @@
       <c r="C3" s="18">
         <v>9</v>
       </c>
-      <c r="E3" s="18">
-        <v>4</v>
-      </c>
-      <c r="F3" s="59">
+      <c r="E3" s="60">
+        <v>4</v>
+      </c>
+      <c r="F3" s="61">
         <v>8</v>
       </c>
       <c r="G3" s="18">
         <v>27</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="60">
         <v>18</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="60">
         <v>9</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="60">
         <v>3</v>
       </c>
       <c r="K3" s="18">
         <v>11</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L3" s="60">
         <v>15</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="60">
         <v>15</v>
       </c>
       <c r="N3" s="18">
         <v>3</v>
       </c>
-      <c r="O3" s="18">
+      <c r="O3" s="60">
         <v>44</v>
       </c>
       <c r="P3" s="18">
@@ -37079,7 +37291,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="18">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" s="18">
         <v>2</v>
@@ -37087,37 +37299,37 @@
       <c r="C4" s="18">
         <v>7</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="60">
         <v>17</v>
       </c>
-      <c r="F4" s="59">
+      <c r="F4" s="61">
         <v>4</v>
       </c>
       <c r="G4" s="18">
         <v>2</v>
       </c>
-      <c r="H4" s="18">
-        <v>5</v>
-      </c>
-      <c r="I4" s="18">
+      <c r="H4" s="60">
+        <v>5</v>
+      </c>
+      <c r="I4" s="60">
         <v>24</v>
       </c>
-      <c r="J4" s="18">
-        <v>31</v>
+      <c r="J4" s="60">
+        <v>32</v>
       </c>
       <c r="K4" s="18">
         <v>34</v>
       </c>
-      <c r="L4" s="18">
-        <v>1</v>
-      </c>
-      <c r="M4" s="18">
+      <c r="L4" s="60">
+        <v>1</v>
+      </c>
+      <c r="M4" s="60">
         <v>26</v>
       </c>
       <c r="N4" s="18">
         <v>0</v>
       </c>
-      <c r="O4" s="18">
+      <c r="O4" s="60">
         <v>17</v>
       </c>
       <c r="P4" s="18">
@@ -37131,34 +37343,34 @@
       <c r="C5" s="18">
         <v>23</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="60">
         <v>15</v>
       </c>
-      <c r="F5" s="59">
+      <c r="F5" s="61">
         <v>1</v>
       </c>
       <c r="G5" s="18">
         <v>5</v>
       </c>
-      <c r="H5" s="18">
-        <v>11</v>
-      </c>
-      <c r="I5" s="18">
+      <c r="H5" s="60">
+        <v>12</v>
+      </c>
+      <c r="I5" s="60">
         <v>11</v>
       </c>
       <c r="K5" s="18">
         <v>12</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="60">
         <v>13</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="60">
         <v>1</v>
       </c>
       <c r="N5" s="18">
         <v>20</v>
       </c>
-      <c r="O5" s="18">
+      <c r="O5" s="60">
         <v>17</v>
       </c>
       <c r="P5" s="18">
@@ -37167,37 +37379,37 @@
     </row>
     <row r="6" spans="1:16">
       <c r="B6" s="18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="18">
         <v>1</v>
       </c>
-      <c r="E6" s="18">
-        <v>0</v>
-      </c>
-      <c r="F6" s="59">
+      <c r="E6" s="60">
+        <v>0</v>
+      </c>
+      <c r="F6" s="61">
         <v>8</v>
       </c>
       <c r="G6" s="18">
         <v>8</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="60">
         <v>0</v>
       </c>
       <c r="K6" s="18">
         <v>13</v>
       </c>
-      <c r="L6" s="18">
-        <v>1</v>
-      </c>
-      <c r="M6" s="18">
+      <c r="L6" s="60">
+        <v>1</v>
+      </c>
+      <c r="M6" s="60">
         <v>7</v>
       </c>
       <c r="N6" s="18">
         <v>12</v>
       </c>
-      <c r="O6" s="18">
-        <v>30</v>
+      <c r="O6" s="60">
+        <v>31</v>
       </c>
       <c r="P6" s="18">
         <v>0</v>
@@ -37207,25 +37419,25 @@
       <c r="C7" s="18">
         <v>0</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="60">
         <v>28</v>
       </c>
-      <c r="F7" s="59">
+      <c r="F7" s="61">
         <v>11</v>
       </c>
       <c r="G7" s="18">
         <v>1</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="60">
         <v>10</v>
       </c>
       <c r="K7" s="18">
         <v>3</v>
       </c>
-      <c r="L7" s="18">
-        <v>0</v>
-      </c>
-      <c r="M7" s="18">
+      <c r="L7" s="60">
+        <v>0</v>
+      </c>
+      <c r="M7" s="60">
         <v>20</v>
       </c>
       <c r="N7" s="18">
@@ -37239,25 +37451,25 @@
       <c r="C8" s="18">
         <v>6</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="60">
         <v>20</v>
       </c>
-      <c r="F8" s="59">
+      <c r="F8" s="61">
         <v>0</v>
       </c>
       <c r="G8" s="18">
         <v>1</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="60">
         <v>21</v>
       </c>
       <c r="K8" s="18">
         <v>2</v>
       </c>
-      <c r="L8" s="18">
-        <v>62</v>
-      </c>
-      <c r="M8" s="18">
+      <c r="L8" s="60">
+        <v>63</v>
+      </c>
+      <c r="M8" s="60">
         <v>0</v>
       </c>
       <c r="N8" s="18">
@@ -37271,78 +37483,81 @@
       <c r="C9" s="18">
         <v>14</v>
       </c>
-      <c r="E9" s="18">
-        <v>18</v>
-      </c>
-      <c r="F9" s="59">
+      <c r="E9" s="60">
+        <v>19</v>
+      </c>
+      <c r="F9" s="61">
         <v>0</v>
       </c>
       <c r="G9" s="18">
         <v>4</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="60">
         <v>7</v>
       </c>
       <c r="K9" s="18">
         <v>12</v>
       </c>
-      <c r="M9" s="18">
-        <v>15</v>
+      <c r="M9" s="60">
+        <v>16</v>
       </c>
       <c r="N9" s="18">
         <v>28</v>
       </c>
       <c r="P9" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="C10" s="18">
         <v>2</v>
       </c>
-      <c r="F10" s="59">
+      <c r="F10" s="61">
         <v>0</v>
       </c>
       <c r="G10" s="18">
         <v>2</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="60">
         <v>5</v>
       </c>
       <c r="K10" s="18">
         <v>1</v>
+      </c>
+      <c r="N10" s="18">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="C11" s="18">
-        <v>24</v>
-      </c>
-      <c r="F11" s="59">
+        <v>25</v>
+      </c>
+      <c r="F11" s="61">
         <v>11</v>
       </c>
       <c r="G11" s="18">
-        <v>2</v>
-      </c>
-      <c r="I11" s="18">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="I11" s="60">
+        <v>8</v>
       </c>
       <c r="K11" s="18">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="F12" s="59">
+      <c r="F12" s="61">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="F13" s="59">
+      <c r="F13" s="61">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="F14" s="59">
-        <v>20</v>
+      <c r="F14" s="61">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -37356,7 +37571,7 @@
   <dimension ref="A2:AG24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -37488,7 +37703,7 @@
     <row r="13" spans="5:13" ht="14.25" customHeight="1"/>
     <row r="14" spans="5:13" s="44" customFormat="1" ht="36" customHeight="1">
       <c r="E14" s="57" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="5:13" ht="36" customHeight="1">
@@ -37576,7 +37791,7 @@
   <dimension ref="A3:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -37587,38 +37802,38 @@
   <sheetData>
     <row r="3" spans="1:2" ht="33" customHeight="1">
       <c r="B3" s="51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="24.75" customHeight="1">
       <c r="B6" s="51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="25.5" customHeight="1">
       <c r="B9" s="51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30.75" customHeight="1">
       <c r="B12" s="51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="28.5" customHeight="1">
       <c r="A15" s="50"/>
       <c r="B15" s="51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="24.75" customHeight="1">
       <c r="B18" s="51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="33.75" customHeight="1">
-      <c r="B21" s="51" t="s">
-        <v>18</v>
+      <c r="B21" s="59" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cp data up && function up
</commit_message>
<xml_diff>
--- a/_back/cp/cp.xlsx
+++ b/_back/cp/cp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -100,10 +100,6 @@
   </si>
   <si>
     <t>关注大趋势</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -364,7 +360,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -407,6 +403,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -420,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -555,6 +557,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -865,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO105"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y71" sqref="Y71"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L68" sqref="L68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.625" defaultRowHeight="13.5"/>
@@ -5080,7 +5088,7 @@
         <v>0</v>
       </c>
       <c r="P42" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q42" s="7">
         <v>0</v>
@@ -5559,7 +5567,7 @@
         <v>12</v>
       </c>
       <c r="J47" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K47" s="7">
         <v>9</v>
@@ -5756,7 +5764,7 @@
       </c>
       <c r="J49" s="7"/>
       <c r="K49" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L49" s="7">
         <v>3</v>
@@ -5811,7 +5819,7 @@
         <v>0</v>
       </c>
       <c r="AD49" s="7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE49" s="7">
         <v>1</v>
@@ -5963,7 +5971,7 @@
         <v>0</v>
       </c>
       <c r="R51" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S51" s="7">
         <v>1</v>
@@ -6006,7 +6014,7 @@
         <v>0</v>
       </c>
       <c r="AG51" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:33" s="3" customFormat="1">
@@ -6062,12 +6070,14 @@
       <c r="T52" s="7">
         <v>7</v>
       </c>
-      <c r="U52" s="7"/>
+      <c r="U52" s="7">
+        <v>0</v>
+      </c>
       <c r="V52" s="7">
         <v>1</v>
       </c>
       <c r="W52" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X52" s="7">
         <v>0</v>
@@ -6097,7 +6107,9 @@
       <c r="AG52" s="7"/>
     </row>
     <row r="53" spans="1:33" s="3" customFormat="1">
-      <c r="A53" s="7"/>
+      <c r="A53" s="7">
+        <v>0</v>
+      </c>
       <c r="B53" s="7">
         <v>1</v>
       </c>
@@ -6131,7 +6143,7 @@
         <v>1</v>
       </c>
       <c r="N53" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O53" s="7">
         <v>5</v>
@@ -6172,7 +6184,7 @@
       </c>
       <c r="AD53" s="7"/>
       <c r="AE53" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AF53" s="7">
         <v>1</v>
@@ -6185,7 +6197,7 @@
         <v>5</v>
       </c>
       <c r="C54" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D54" s="7">
         <v>1</v>
@@ -6226,7 +6238,7 @@
         <v>0</v>
       </c>
       <c r="T54" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U54" s="7"/>
       <c r="V54" s="7">
@@ -6237,7 +6249,7 @@
         <v>0</v>
       </c>
       <c r="Y54" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Z54" s="7">
         <v>5</v>
@@ -6249,7 +6261,7 @@
         <v>3</v>
       </c>
       <c r="AC54" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AD54" s="7"/>
       <c r="AE54" s="7"/>
@@ -6278,7 +6290,7 @@
       </c>
       <c r="H55" s="7"/>
       <c r="I55" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
@@ -6323,7 +6335,7 @@
       <c r="AD55" s="7"/>
       <c r="AE55" s="7"/>
       <c r="AF55" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AG55" s="7"/>
     </row>
@@ -6365,7 +6377,7 @@
       </c>
       <c r="R56" s="7"/>
       <c r="S56" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T56" s="7"/>
       <c r="U56" s="7"/>
@@ -6381,7 +6393,7 @@
         <v>4</v>
       </c>
       <c r="AA56" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB56" s="7">
         <v>0</v>
@@ -6413,7 +6425,9 @@
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
       <c r="K57" s="7"/>
-      <c r="L57" s="7"/>
+      <c r="L57" s="7">
+        <v>0</v>
+      </c>
       <c r="M57" s="7">
         <v>15</v>
       </c>
@@ -6520,10 +6534,10 @@
         <v>0</v>
       </c>
       <c r="F59" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G59" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M59" s="7">
         <v>4</v>
@@ -6565,7 +6579,7 @@
         <v>2</v>
       </c>
       <c r="O60" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q60" s="7">
         <v>4</v>
@@ -6588,7 +6602,7 @@
     <row r="61" spans="1:33" s="14" customFormat="1">
       <c r="A61" s="7"/>
       <c r="B61" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C61" s="26"/>
       <c r="D61" s="7">
@@ -6621,7 +6635,7 @@
       </c>
       <c r="W61" s="7"/>
       <c r="X61" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y61" s="7"/>
       <c r="Z61" s="7">
@@ -6666,7 +6680,9 @@
       <c r="S62" s="4"/>
       <c r="T62" s="7"/>
       <c r="U62" s="7"/>
-      <c r="V62" s="7"/>
+      <c r="V62" s="7">
+        <v>0</v>
+      </c>
       <c r="W62" s="7"/>
       <c r="X62" s="7"/>
       <c r="Y62" s="7"/>
@@ -6675,7 +6691,7 @@
       </c>
       <c r="AA62" s="26"/>
       <c r="AB62" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC62" s="7"/>
       <c r="AD62" s="7"/>
@@ -6716,7 +6732,7 @@
       <c r="X63" s="4"/>
       <c r="Y63" s="4"/>
       <c r="Z63" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AA63" s="26"/>
       <c r="AB63" s="7"/>
@@ -6766,7 +6782,9 @@
       <c r="D65" s="3">
         <v>0</v>
       </c>
-      <c r="E65" s="4"/>
+      <c r="E65" s="4">
+        <v>0</v>
+      </c>
       <c r="F65" s="7"/>
       <c r="H65" s="4"/>
       <c r="J65" s="3"/>
@@ -6779,7 +6797,7 @@
       <c r="O65" s="4"/>
       <c r="P65" s="4"/>
       <c r="Q65" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R65" s="4"/>
       <c r="S65" s="4"/>
@@ -6806,7 +6824,9 @@
       <c r="I66" s="4"/>
       <c r="J66" s="3"/>
       <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
+      <c r="M66" s="4">
+        <v>0</v>
+      </c>
       <c r="N66" s="4"/>
       <c r="O66" s="4"/>
       <c r="Q66" s="4"/>
@@ -6827,7 +6847,7 @@
     </row>
     <row r="67" spans="1:33">
       <c r="D67" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E67" s="14"/>
       <c r="F67" s="4"/>
@@ -6880,16 +6900,8 @@
       <c r="AF68" s="39"/>
       <c r="AG68" s="5"/>
     </row>
-    <row r="69" spans="1:33" s="45" customFormat="1">
-      <c r="M69" s="45" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="70" spans="1:33" s="43" customFormat="1">
-      <c r="E70" s="43" t="s">
-        <v>21</v>
-      </c>
-    </row>
+    <row r="69" spans="1:33" s="45" customFormat="1"/>
+    <row r="70" spans="1:33" s="43" customFormat="1"/>
     <row r="71" spans="1:33" s="47" customFormat="1"/>
     <row r="72" spans="1:33">
       <c r="C72" s="5"/>
@@ -7563,8 +7575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT978"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S136" sqref="S136"/>
+    <sheetView topLeftCell="A113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G145" sqref="G145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5"/>
@@ -16573,7 +16585,7 @@
         <v>2</v>
       </c>
       <c r="V119" s="23">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W119" s="23"/>
       <c r="X119" s="22">
@@ -16982,7 +16994,7 @@
         <v>0</v>
       </c>
       <c r="V124" s="23">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="W124" s="23"/>
       <c r="X124" s="22">
@@ -17277,7 +17289,7 @@
       </c>
       <c r="P127" s="22"/>
       <c r="Q127" s="23">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R127" s="22">
         <v>2</v>
@@ -17478,14 +17490,14 @@
         <v>28</v>
       </c>
       <c r="P129" s="22"/>
-      <c r="Q129" s="23">
+      <c r="Q129" s="64">
         <v>10</v>
       </c>
       <c r="R129" s="22">
         <v>1</v>
       </c>
       <c r="S129" s="23">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T129" s="22">
         <v>6</v>
@@ -17509,7 +17521,9 @@
       <c r="AA129" s="22">
         <v>6</v>
       </c>
-      <c r="AB129" s="23"/>
+      <c r="AB129" s="19">
+        <v>10</v>
+      </c>
       <c r="AC129" s="23"/>
       <c r="AD129" s="23"/>
       <c r="AF129" s="23"/>
@@ -17580,7 +17594,7 @@
         <v>3</v>
       </c>
       <c r="R130" s="23">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="S130" s="22">
         <v>7</v>
@@ -17592,7 +17606,7 @@
         <v>4</v>
       </c>
       <c r="V130" s="23">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="W130" s="23"/>
       <c r="X130" s="22">
@@ -17777,7 +17791,7 @@
       </c>
       <c r="P132" s="22"/>
       <c r="Q132" s="23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R132" s="22">
         <v>6</v>
@@ -17882,13 +17896,13 @@
       <c r="R133" s="22">
         <v>5</v>
       </c>
-      <c r="S133" s="23">
+      <c r="S133" s="64">
         <v>6</v>
       </c>
       <c r="T133" s="22">
         <v>0</v>
       </c>
-      <c r="U133" s="23">
+      <c r="U133" s="64">
         <v>6</v>
       </c>
       <c r="V133" s="22">
@@ -17907,8 +17921,12 @@
       <c r="AA133" s="19">
         <v>5</v>
       </c>
-      <c r="AB133" s="23"/>
-      <c r="AC133" s="23"/>
+      <c r="AB133" s="19">
+        <v>6</v>
+      </c>
+      <c r="AC133" s="19">
+        <v>6</v>
+      </c>
       <c r="AD133" s="41"/>
       <c r="AF133" s="41"/>
       <c r="AH133" s="21">
@@ -17968,7 +17986,7 @@
         <v>23</v>
       </c>
       <c r="P134" s="22"/>
-      <c r="Q134" s="23">
+      <c r="Q134" s="64">
         <v>5</v>
       </c>
       <c r="R134" s="22">
@@ -18002,7 +18020,9 @@
       <c r="AB134" s="22">
         <v>2</v>
       </c>
-      <c r="AC134" s="23"/>
+      <c r="AC134" s="19">
+        <v>5</v>
+      </c>
       <c r="AD134" s="41"/>
       <c r="AF134" s="41"/>
       <c r="AH134" s="21">
@@ -18069,7 +18089,7 @@
       </c>
       <c r="P135" s="22"/>
       <c r="Q135" s="23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R135" s="22">
         <v>1</v>
@@ -18078,13 +18098,13 @@
         <v>1</v>
       </c>
       <c r="T135" s="23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U135" s="23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="V135" s="23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W135" s="23"/>
       <c r="X135" s="21">
@@ -18166,19 +18186,19 @@
         <v>0</v>
       </c>
       <c r="R136" s="23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S136" s="23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T136" s="22">
         <v>1</v>
       </c>
       <c r="U136" s="23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V136" s="23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W136" s="23"/>
       <c r="X136" s="21">
@@ -18260,13 +18280,13 @@
         <v>0</v>
       </c>
       <c r="R137" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S137" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T137" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U137" s="22">
         <v>0</v>
@@ -18352,22 +18372,22 @@
         <v>12</v>
       </c>
       <c r="Q138" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R138" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S138" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T138" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U138" s="19">
         <v>0</v>
       </c>
       <c r="V138" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W138" s="15"/>
       <c r="X138" s="16">
@@ -18440,26 +18460,30 @@
       </c>
       <c r="P139" s="22"/>
       <c r="Q139" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R139" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S139" s="20">
-        <v>0</v>
-      </c>
-      <c r="T139" s="20">
-        <v>0</v>
-      </c>
-      <c r="U139" s="20">
+        <v>1</v>
+      </c>
+      <c r="T139" s="63">
+        <v>0</v>
+      </c>
+      <c r="U139" s="63">
         <v>0</v>
       </c>
       <c r="V139" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W139" s="20"/>
-      <c r="X139" s="15"/>
-      <c r="Y139" s="15"/>
+      <c r="X139" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y139" s="16">
+        <v>0</v>
+      </c>
       <c r="Z139" s="15"/>
       <c r="AA139" s="20"/>
       <c r="AB139" s="20"/>
@@ -18495,13 +18519,61 @@
       </c>
     </row>
     <row r="140" spans="1:46" s="21" customFormat="1">
+      <c r="A140" s="21">
+        <v>5</v>
+      </c>
+      <c r="B140" s="21">
+        <v>10</v>
+      </c>
+      <c r="C140" s="21">
+        <v>6</v>
+      </c>
+      <c r="D140" s="21">
+        <v>0</v>
+      </c>
+      <c r="E140" s="21">
+        <v>0</v>
+      </c>
+      <c r="F140" s="21">
+        <v>6</v>
+      </c>
+      <c r="I140" s="21">
+        <v>0</v>
+      </c>
+      <c r="J140" s="21">
+        <v>0</v>
+      </c>
+      <c r="K140" s="21">
+        <v>5</v>
+      </c>
+      <c r="L140" s="21">
+        <v>6</v>
+      </c>
+      <c r="M140" s="21">
+        <v>6</v>
+      </c>
+      <c r="N140" s="21">
+        <v>10</v>
+      </c>
       <c r="P140" s="22"/>
-      <c r="Q140" s="20"/>
-      <c r="R140" s="20"/>
-      <c r="S140" s="20"/>
-      <c r="T140" s="20"/>
-      <c r="U140" s="20"/>
-      <c r="V140" s="20"/>
+      <c r="Q140" s="20">
+        <v>0</v>
+      </c>
+      <c r="R140" s="20">
+        <v>0</v>
+      </c>
+      <c r="S140" s="20">
+        <v>0</v>
+      </c>
+      <c r="T140" s="20">
+        <v>0</v>
+      </c>
+      <c r="U140" s="20">
+        <v>0</v>
+      </c>
+      <c r="V140" s="20">
+        <v>0</v>
+      </c>
       <c r="W140" s="20"/>
       <c r="X140" s="15"/>
       <c r="Y140" s="15"/>
@@ -18511,6 +18583,27 @@
       <c r="AC140" s="15"/>
       <c r="AD140" s="15"/>
       <c r="AF140" s="41"/>
+      <c r="AH140" s="21">
+        <v>0</v>
+      </c>
+      <c r="AI140" s="21">
+        <v>5</v>
+      </c>
+      <c r="AJ140" s="21">
+        <v>6</v>
+      </c>
+      <c r="AK140" s="21">
+        <v>10</v>
+      </c>
+      <c r="AO140" s="21">
+        <v>4</v>
+      </c>
+      <c r="AP140" s="21">
+        <v>0</v>
+      </c>
+      <c r="AQ140" s="21">
+        <v>0</v>
+      </c>
     </row>
     <row r="141" spans="1:46" s="21" customFormat="1">
       <c r="P141" s="22"/>
@@ -31602,7 +31695,7 @@
   <dimension ref="A1:AO205"/>
   <sheetViews>
     <sheetView topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N143" sqref="N143"/>
+      <selection activeCell="L144" sqref="L144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.625" defaultRowHeight="13.5"/>
@@ -34491,13 +34584,22 @@
       </c>
     </row>
     <row r="140" spans="1:29">
-      <c r="A140" s="10"/>
+      <c r="A140" s="11">
+        <v>2</v>
+      </c>
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
       <c r="D140" s="10"/>
       <c r="E140" s="10"/>
-      <c r="F140" s="10"/>
-      <c r="G140" s="10"/>
+      <c r="F140" s="9">
+        <v>1</v>
+      </c>
+      <c r="G140" s="11">
+        <v>2</v>
+      </c>
+      <c r="K140" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="141" spans="1:29">
       <c r="A141" s="10"/>
@@ -34926,7 +35028,7 @@
   <dimension ref="A1:U198"/>
   <sheetViews>
     <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="R143" sqref="R143"/>
+      <selection activeCell="I145" sqref="I145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -37759,6 +37861,53 @@
         <v>15</v>
       </c>
     </row>
+    <row r="140" spans="1:21">
+      <c r="A140" s="1">
+        <v>2</v>
+      </c>
+      <c r="B140" s="1">
+        <v>2</v>
+      </c>
+      <c r="C140" s="1">
+        <v>2</v>
+      </c>
+      <c r="F140" s="1">
+        <v>2</v>
+      </c>
+      <c r="G140" s="1">
+        <v>0</v>
+      </c>
+      <c r="H140" s="1">
+        <v>1</v>
+      </c>
+      <c r="I140" s="1">
+        <v>1</v>
+      </c>
+      <c r="J140" s="1">
+        <v>2</v>
+      </c>
+      <c r="K140" s="1">
+        <v>0</v>
+      </c>
+      <c r="N140" s="1">
+        <v>0</v>
+      </c>
+      <c r="O140" s="1">
+        <v>1</v>
+      </c>
+      <c r="P140" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q140" s="1">
+        <v>6</v>
+      </c>
+      <c r="R140" s="1">
+        <v>7</v>
+      </c>
+      <c r="S140" s="1">
+        <v>10</v>
+      </c>
+    </row>
     <row r="147" spans="1:19">
       <c r="A147" s="37"/>
       <c r="B147" s="37"/>
@@ -37853,10 +38002,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A100:AN139"/>
+  <dimension ref="A100:AN140"/>
   <sheetViews>
     <sheetView topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="H147" sqref="H147"/>
+      <selection activeCell="I148" sqref="I148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -40009,6 +40158,41 @@
         <v>8</v>
       </c>
     </row>
+    <row r="140" spans="1:23">
+      <c r="A140" s="11">
+        <v>2</v>
+      </c>
+      <c r="B140" s="11">
+        <v>2</v>
+      </c>
+      <c r="C140" s="9">
+        <v>1</v>
+      </c>
+      <c r="E140" s="9">
+        <v>1</v>
+      </c>
+      <c r="L140" s="16">
+        <v>1</v>
+      </c>
+      <c r="M140" s="16">
+        <v>1</v>
+      </c>
+      <c r="N140" s="16">
+        <v>2</v>
+      </c>
+      <c r="O140" s="16">
+        <v>2</v>
+      </c>
+      <c r="P140" s="16">
+        <v>3</v>
+      </c>
+      <c r="Q140" s="16">
+        <v>5</v>
+      </c>
+      <c r="S140" s="16">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -40021,7 +40205,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -40094,7 +40278,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="18">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E2" s="18">
         <v>1</v>
@@ -40229,7 +40413,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="18">
         <v>57</v>
@@ -40276,7 +40460,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="B6" s="18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="19">
         <v>1</v>
@@ -40312,7 +40496,7 @@
         <v>12</v>
       </c>
       <c r="O6" s="18">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="P6" s="18">
         <v>0</v>
@@ -40336,6 +40520,9 @@
       </c>
       <c r="I7" s="18">
         <v>10</v>
+      </c>
+      <c r="J7" s="18">
+        <v>0</v>
       </c>
       <c r="K7" s="18">
         <v>3</v>
@@ -40367,7 +40554,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="18">
         <v>21</v>
@@ -40393,7 +40580,7 @@
         <v>14</v>
       </c>
       <c r="E9" s="18">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F9" s="19">
         <v>0</v>
@@ -40411,13 +40598,13 @@
         <v>2</v>
       </c>
       <c r="M9" s="18">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N9" s="18">
         <v>28</v>
       </c>
       <c r="P9" s="18">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -40437,7 +40624,7 @@
         <v>1</v>
       </c>
       <c r="L10" s="18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N10" s="18">
         <v>1</v>
@@ -40451,27 +40638,27 @@
         <v>11</v>
       </c>
       <c r="G11" s="18">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I11" s="18">
         <v>11</v>
       </c>
       <c r="K11" s="18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N11" s="18">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="C12" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="19">
         <v>9</v>
       </c>
       <c r="I12" s="18">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -40486,7 +40673,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="F15" s="19">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>